<commit_message>
Added assertions to TCs
</commit_message>
<xml_diff>
--- a/com.att/src/test/resources/test_data.xlsx
+++ b/com.att/src/test/resources/test_data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zohralamrani/IdeaProjects/Team1SeleniumBootcamp/com.att/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5BA561-1FED-4947-A0ED-575038A32F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68522184-B9E3-2E4B-A5DC-652D9EDF8DA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13580" yWindow="1000" windowWidth="17240" windowHeight="16680" xr2:uid="{7101F360-28F6-4A46-B2C7-3953E0E4AC55}"/>
+    <workbookView xWindow="14560" yWindow="1020" windowWidth="17240" windowHeight="16680" activeTab="1" xr2:uid="{7101F360-28F6-4A46-B2C7-3953E0E4AC55}"/>
   </bookViews>
   <sheets>
     <sheet name="phonesAndDevices" sheetId="1" r:id="rId1"/>
+    <sheet name="attSearchResultPagePromoMessage" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,12 +36,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Showing pricing with trade-in </t>
   </si>
   <si>
     <t>phonesAndDevicesAssert</t>
+  </si>
+  <si>
+    <t>att search results test assert</t>
+  </si>
+  <si>
+    <t>Shop the latest offers designed for individual first responders and those that support them. See how FirstNet can help save you money.</t>
   </si>
 </sst>
 </file>
@@ -400,7 +407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C22389BD-BB3A-E843-B77C-04C37BD6D3BF}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -420,4 +427,29 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{934D9675-13DB-0548-9915-AD5A9BAE3518}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>